<commit_message>
add the experiment for security monitor
</commit_message>
<xml_diff>
--- a/benchmark/results-3rd.xlsx
+++ b/benchmark/results-3rd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t xml:space="preserve">chartjs-NORMAL</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t xml:space="preserve">initialization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average (ms)</t>
   </si>
   <si>
     <t xml:space="preserve">average (us)</t>
@@ -993,11 +990,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="1299210"/>
-        <c:axId val="47174647"/>
+        <c:axId val="87022874"/>
+        <c:axId val="56210642"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1299210"/>
+        <c:axId val="87022874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,14 +1038,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47174647"/>
+        <c:crossAx val="56210642"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47174647"/>
+        <c:axId val="56210642"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1098,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1299210"/>
+        <c:crossAx val="87022874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1149,9 +1146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>282240</xdr:colOff>
+      <xdr:colOff>281880</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1160,8 +1157,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628920" y="267840"/>
-          <a:ext cx="8054280" cy="7052760"/>
+          <a:off x="619560" y="267840"/>
+          <a:ext cx="7929720" cy="7052400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3163,9 +3160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>416520</xdr:colOff>
+      <xdr:colOff>416160</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3173,8 +3170,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9082800" y="3905280"/>
-        <a:ext cx="7716600" cy="3239280"/>
+        <a:off x="9511560" y="3905280"/>
+        <a:ext cx="8039880" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3194,13 +3191,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3226,6 +3223,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -10067,7 +10067,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10929,7 +10929,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11937,15 +11937,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13758,7 +13758,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16182,17 +16182,17 @@
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16247,49 +16247,49 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.008971</v>
+        <v>8.971</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.011163</v>
+        <v>11.163</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.011483</v>
+        <v>11.483</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0.020575</v>
+        <v>20.575</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.009649</v>
+        <v>9.649</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.011055</v>
+        <v>11.055</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>0.009701</v>
+        <v>9.701</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0.010204</v>
+        <v>10.204</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0.009343</v>
+        <v>9.343</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>0.009453</v>
+        <v>9.453</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>0.02354</v>
+        <v>23.54</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>0.023587</v>
+        <v>23.587</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>0.00463</v>
+        <v>4.63</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>0.006037</v>
+        <v>6.037</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>13.7</v>
+        <v>13700</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16297,49 +16297,49 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.011796</v>
+        <v>11.796</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.011897</v>
+        <v>11.897</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.00828</v>
+        <v>8.28</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0.020989</v>
+        <v>20.989</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.012051</v>
+        <v>12.051</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.013444</v>
+        <v>13.444</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0.013124</v>
+        <v>13.124</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0.012118</v>
+        <v>12.118</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.009018</v>
+        <v>9.018</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0.011984</v>
+        <v>11.984</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0.022701</v>
+        <v>22.701</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>0.021826</v>
+        <v>21.826</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>0.00221</v>
+        <v>2.21</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>0.005914</v>
+        <v>5.914</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>3.049</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16347,49 +16347,49 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.012856</v>
+        <v>12.856</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.010219</v>
+        <v>10.219</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.010093</v>
+        <v>10.093</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.02055</v>
+        <v>20.55</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.010019</v>
+        <v>10.019</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.011185</v>
+        <v>11.185</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.009974</v>
+        <v>9.974</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.013153</v>
+        <v>13.153</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.011145</v>
+        <v>11.145</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>0.012456</v>
+        <v>12.456</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0.022781</v>
+        <v>22.781</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>0.024841</v>
+        <v>24.841</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>0.004351</v>
+        <v>4.351</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>0.006455</v>
+        <v>6.455</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>5.261</v>
+        <v>5261</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16397,49 +16397,49 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.009374</v>
+        <v>9.374</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.011066</v>
+        <v>11.066</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.01103</v>
+        <v>11.03</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.023296</v>
+        <v>23.296</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.00947</v>
+        <v>9.47</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.012469</v>
+        <v>12.469</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.012887</v>
+        <v>12.887</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.012593</v>
+        <v>12.593</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.0101</v>
+        <v>10.1</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.013714</v>
+        <v>13.714</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.022469</v>
+        <v>22.469</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>0.026482</v>
+        <v>26.482</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>0.002364</v>
+        <v>2.364</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>0.00743</v>
+        <v>7.43</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>36.166</v>
+        <v>36166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16447,49 +16447,49 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.011849</v>
+        <v>11.849</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.010595</v>
+        <v>10.595</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.011541</v>
+        <v>11.541</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.021567</v>
+        <v>21.567</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.011715</v>
+        <v>11.715</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.010899</v>
+        <v>10.899</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.009383</v>
+        <v>9.383</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.011768</v>
+        <v>11.768</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.010499</v>
+        <v>10.499</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>0.007179</v>
+        <v>7.179</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0.021063</v>
+        <v>21.063</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>0.02451</v>
+        <v>24.51</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>0.004524</v>
+        <v>4.524</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>0.006261</v>
+        <v>6.261</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>48.792</v>
+        <v>48792</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16497,49 +16497,49 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.009765</v>
+        <v>9.765</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.012007</v>
+        <v>12.007</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.010059</v>
+        <v>10.059</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.01894</v>
+        <v>18.94</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.011008</v>
+        <v>11.008</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.009204</v>
+        <v>9.204</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.010747</v>
+        <v>10.747</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.01059</v>
+        <v>10.59</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.011514</v>
+        <v>11.514</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>0.010881</v>
+        <v>10.881</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0.023548</v>
+        <v>23.548</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>0.024334</v>
+        <v>24.334</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>0.004392</v>
+        <v>4.392</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>0.005915</v>
+        <v>5.915</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>41.868</v>
+        <v>41868</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16547,49 +16547,49 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.010349</v>
+        <v>10.349</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.012591</v>
+        <v>12.591</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.011269</v>
+        <v>11.269</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>0.021095</v>
+        <v>21.095</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.010287</v>
+        <v>10.287</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.012125</v>
+        <v>12.125</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.013094</v>
+        <v>13.094</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0.011019</v>
+        <v>11.019</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.012495</v>
+        <v>12.495</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>0.009812</v>
+        <v>9.812</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0.020779</v>
+        <v>20.779</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>0.025159</v>
+        <v>25.159</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>0.00342</v>
+        <v>3.42</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>0.006036</v>
+        <v>6.036</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>12.637</v>
+        <v>12637</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16597,49 +16597,49 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.011046</v>
+        <v>11.046</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.010431</v>
+        <v>10.431</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.012096</v>
+        <v>12.096</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0.021897</v>
+        <v>21.897</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.009027</v>
+        <v>9.027</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.010451</v>
+        <v>10.451</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.01223</v>
+        <v>12.23</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0.010828</v>
+        <v>10.828</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.009425</v>
+        <v>9.425</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>0.009392</v>
+        <v>9.392</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0.019941</v>
+        <v>19.941</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>0.022124</v>
+        <v>22.124</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>0.004446</v>
+        <v>4.446</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>0.006234</v>
+        <v>6.234</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>4.736</v>
+        <v>4736</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16647,49 +16647,49 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.009065</v>
+        <v>9.065</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.010597</v>
+        <v>10.597</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.009324</v>
+        <v>9.324</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>0.023606</v>
+        <v>23.606</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.009096</v>
+        <v>9.096</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.012005</v>
+        <v>12.005</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.011868</v>
+        <v>11.868</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0.013152</v>
+        <v>13.152</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.012503</v>
+        <v>12.503</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0.011555</v>
+        <v>11.555</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0.0208</v>
+        <v>20.8</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>0.024091</v>
+        <v>24.091</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>0.002393</v>
+        <v>2.393</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>0.006548</v>
+        <v>6.548</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>15.382</v>
+        <v>15382</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16697,49 +16697,49 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.010101</v>
+        <v>10.101</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.012553</v>
+        <v>12.553</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.007957</v>
+        <v>7.957</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>0.02387</v>
+        <v>23.87</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.008998</v>
+        <v>8.998</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.013022</v>
+        <v>13.022</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.011957</v>
+        <v>11.957</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0.011837</v>
+        <v>11.837</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.010438</v>
+        <v>10.438</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0.010941</v>
+        <v>10.941</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0.021718</v>
+        <v>21.718</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>0.023406</v>
+        <v>23.406</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>0.004028</v>
+        <v>4.028</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>0.007622</v>
+        <v>7.622</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>29.19</v>
+        <v>29190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16747,49 +16747,49 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.011886</v>
+        <v>11.886</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.010855</v>
+        <v>10.855</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.012133</v>
+        <v>12.133</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>0.022347</v>
+        <v>22.347</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.010263</v>
+        <v>10.263</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.011851</v>
+        <v>11.851</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.010939</v>
+        <v>10.939</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0.011077</v>
+        <v>11.077</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.010377</v>
+        <v>10.377</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>0.012424</v>
+        <v>12.424</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>0.023114</v>
+        <v>23.114</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>0.025827</v>
+        <v>25.827</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>0.003021</v>
+        <v>3.021</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>0.007087</v>
+        <v>7.087</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>9.794</v>
+        <v>9794</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16797,49 +16797,49 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.011453</v>
+        <v>11.453</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0.010842</v>
+        <v>10.842</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.009768</v>
+        <v>9.768</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0.021999</v>
+        <v>21.999</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.011304</v>
+        <v>11.304</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.011816</v>
+        <v>11.816</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.010798</v>
+        <v>10.798</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.011093</v>
+        <v>11.093</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.010543</v>
+        <v>10.543</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>0.011806</v>
+        <v>11.806</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0.022158</v>
+        <v>22.158</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>0.019251</v>
+        <v>19.251</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>0.003629</v>
+        <v>3.629</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>0.007389</v>
+        <v>7.389</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>30.531</v>
+        <v>30531</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16847,49 +16847,49 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.008974</v>
+        <v>8.974</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.009247</v>
+        <v>9.247</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.010278</v>
+        <v>10.278</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>0.02215</v>
+        <v>22.15</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.010112</v>
+        <v>10.112</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.01116</v>
+        <v>11.16</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.013254</v>
+        <v>13.254</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0.009378</v>
+        <v>9.378</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.011309</v>
+        <v>11.309</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>0.011228</v>
+        <v>11.228</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.021605</v>
+        <v>21.605</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>0.022579</v>
+        <v>22.579</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>0.004518</v>
+        <v>4.518</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>0.008565</v>
+        <v>8.565</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>16.295</v>
+        <v>16295</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16897,49 +16897,49 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.013214</v>
+        <v>13.214</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0.011276</v>
+        <v>11.276</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.010446</v>
+        <v>10.446</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>0.020526</v>
+        <v>20.526</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.010592</v>
+        <v>10.592</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.012379</v>
+        <v>12.379</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.010664</v>
+        <v>10.664</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>0.013313</v>
+        <v>13.313</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.011247</v>
+        <v>11.247</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>0.010715</v>
+        <v>10.715</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0.022702</v>
+        <v>22.702</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>0.02311</v>
+        <v>23.11</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>0.004537</v>
+        <v>4.537</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>0.007395</v>
+        <v>7.395</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>13.265</v>
+        <v>13265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16947,49 +16947,49 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.009483</v>
+        <v>9.483</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.012103</v>
+        <v>12.103</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.012222</v>
+        <v>12.222</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0.022521</v>
+        <v>22.521</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.012299</v>
+        <v>12.299</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.012328</v>
+        <v>12.328</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.013034</v>
+        <v>13.034</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>0.013348</v>
+        <v>13.348</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.011027</v>
+        <v>11.027</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>0.011227</v>
+        <v>11.227</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0.02276</v>
+        <v>22.76</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>0.022268</v>
+        <v>22.268</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>0.004453</v>
+        <v>4.453</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>0.007149</v>
+        <v>7.149</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>21.795</v>
+        <v>21795</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16997,49 +16997,49 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.012551</v>
+        <v>12.551</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.01008</v>
+        <v>10.08</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.009851</v>
+        <v>9.851</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>0.02435</v>
+        <v>24.35</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.010818</v>
+        <v>10.818</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.010168</v>
+        <v>10.168</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.008784</v>
+        <v>8.784</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0.010016</v>
+        <v>10.016</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.011153</v>
+        <v>11.153</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0.012134</v>
+        <v>12.134</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>0.023742</v>
+        <v>23.742</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>0.020438</v>
+        <v>20.438</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>0.00476</v>
+        <v>4.76</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>0.00714</v>
+        <v>7.14</v>
       </c>
       <c r="P17" s="0" t="n">
-        <v>26.15</v>
+        <v>26150</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17047,49 +17047,49 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.009508</v>
+        <v>9.508</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.012277</v>
+        <v>12.277</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.009095</v>
+        <v>9.095</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>0.019498</v>
+        <v>19.498</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.01384</v>
+        <v>13.84</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.011149</v>
+        <v>11.149</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.010862</v>
+        <v>10.862</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>0.010329</v>
+        <v>10.329</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.010887</v>
+        <v>10.887</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0.009852</v>
+        <v>9.852</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>0.022541</v>
+        <v>22.541</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>0.023906</v>
+        <v>23.906</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>0.002966</v>
+        <v>2.966</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>0.007805</v>
+        <v>7.805</v>
       </c>
       <c r="P18" s="0" t="n">
-        <v>5.021</v>
+        <v>5021</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17097,49 +17097,49 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.009436</v>
+        <v>9.436</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.011337</v>
+        <v>11.337</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.013307</v>
+        <v>13.307</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0.025053</v>
+        <v>25.053</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.010841</v>
+        <v>10.841</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.010158</v>
+        <v>10.158</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.011614</v>
+        <v>11.614</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>0.010792</v>
+        <v>10.792</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.010584</v>
+        <v>10.584</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0.009252</v>
+        <v>9.252</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>0.022764</v>
+        <v>22.764</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>0.021628</v>
+        <v>21.628</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>0.003181</v>
+        <v>3.181</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>0.007084</v>
+        <v>7.084</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>7.105</v>
+        <v>7105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17147,49 +17147,49 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.00842</v>
+        <v>8.42</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.014271</v>
+        <v>14.271</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.009403</v>
+        <v>9.403</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>0.020976</v>
+        <v>20.976</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.011679</v>
+        <v>11.679</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.013916</v>
+        <v>13.916</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.011429</v>
+        <v>11.429</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>0.012352</v>
+        <v>12.352</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.008825</v>
+        <v>8.825</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>0.011175</v>
+        <v>11.175</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>0.025089</v>
+        <v>25.089</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>0.025305</v>
+        <v>25.305</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>0.004848</v>
+        <v>4.848</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>0.007186</v>
+        <v>7.186</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>7.266</v>
+        <v>7266</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17197,175 +17197,114 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.009995</v>
+        <v>9.995</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0.010334</v>
+        <v>10.334</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.008635</v>
+        <v>8.635</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>0.021909</v>
+        <v>21.909</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0.014624</v>
+        <v>14.624</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.007407</v>
+        <v>7.407</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0.011595</v>
+        <v>11.595</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>0.011675</v>
+        <v>11.675</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.013541</v>
+        <v>13.541</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>0.007806</v>
+        <v>7.806</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>0.026984</v>
+        <v>26.984</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>0.021408</v>
+        <v>21.408</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>0.004439</v>
+        <v>4.439</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>0.007414</v>
+        <v>7.414</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>24.026</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">AVERAGE(B2:B21)</f>
-        <v>0.0105046</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <f aca="false">AVERAGE(C2:C21)</f>
-        <v>0.01128705</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <f aca="false">AVERAGE(D2:D21)</f>
-        <v>0.0104135</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <f aca="false">AVERAGE(E2:E21)</f>
-        <v>0.0218857</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <f aca="false">AVERAGE(F2:F21)</f>
-        <v>0.0108846</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">AVERAGE(G2:G21)</f>
-        <v>0.01140955</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <f aca="false">AVERAGE(H2:H21)</f>
-        <v>0.0113969</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <f aca="false">AVERAGE(I2:I21)</f>
-        <v>0.01153175</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <f aca="false">AVERAGE(J2:J21)</f>
-        <v>0.01079865</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <f aca="false">AVERAGE(K2:K21)</f>
-        <v>0.0107493</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <f aca="false">AVERAGE(L2:L21)</f>
-        <v>0.02263995</v>
-      </c>
-      <c r="M24" s="0" t="n">
-        <f aca="false">AVERAGE(M2:M21)</f>
-        <v>0.023304</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <f aca="false">AVERAGE(N2:N21)</f>
-        <v>0.0038555</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <f aca="false">AVERAGE(O2:O21)</f>
-        <v>0.0069333</v>
-      </c>
-      <c r="P24" s="0" t="n">
-        <f aca="false">AVERAGE(P2:P21)</f>
-        <v>18.60145</v>
+        <v>24026</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="0" t="n">
-        <f aca="false">B24*1000</f>
+        <f aca="false">AVERAGE(B2:B21)</f>
         <v>10.5046</v>
       </c>
       <c r="C25" s="0" t="n">
-        <f aca="false">C24*1000</f>
+        <f aca="false">AVERAGE(C2:C21)</f>
         <v>11.28705</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">D24*1000</f>
+        <f aca="false">AVERAGE(D2:D21)</f>
         <v>10.4135</v>
       </c>
       <c r="E25" s="0" t="n">
-        <f aca="false">E24*1000</f>
+        <f aca="false">AVERAGE(E2:E21)</f>
         <v>21.8857</v>
       </c>
       <c r="F25" s="0" t="n">
-        <f aca="false">F24*1000</f>
+        <f aca="false">AVERAGE(F2:F21)</f>
         <v>10.8846</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">G24*1000</f>
+        <f aca="false">AVERAGE(G2:G21)</f>
         <v>11.40955</v>
       </c>
       <c r="H25" s="0" t="n">
-        <f aca="false">H24*1000</f>
+        <f aca="false">AVERAGE(H2:H21)</f>
         <v>11.3969</v>
       </c>
       <c r="I25" s="0" t="n">
-        <f aca="false">I24*1000</f>
+        <f aca="false">AVERAGE(I2:I21)</f>
         <v>11.53175</v>
       </c>
       <c r="J25" s="0" t="n">
-        <f aca="false">J24*1000</f>
+        <f aca="false">AVERAGE(J2:J21)</f>
         <v>10.79865</v>
       </c>
       <c r="K25" s="0" t="n">
-        <f aca="false">K24*1000</f>
+        <f aca="false">AVERAGE(K2:K21)</f>
         <v>10.7493</v>
       </c>
       <c r="L25" s="0" t="n">
-        <f aca="false">L24*1000</f>
+        <f aca="false">AVERAGE(L2:L21)</f>
         <v>22.63995</v>
       </c>
       <c r="M25" s="0" t="n">
-        <f aca="false">M24*1000</f>
+        <f aca="false">AVERAGE(M2:M21)</f>
         <v>23.304</v>
       </c>
       <c r="N25" s="0" t="n">
-        <f aca="false">N24*1000</f>
+        <f aca="false">AVERAGE(N2:N21)</f>
         <v>3.8555</v>
       </c>
       <c r="O25" s="0" t="n">
-        <f aca="false">O24*1000</f>
+        <f aca="false">AVERAGE(O2:O21)</f>
         <v>6.9333</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <f aca="false">AVERAGE(P2:P21)</f>
+        <v>18601.45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17408,7 +17347,7 @@
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">F25/B25-1</f>
-        <v>0.0361746282580961</v>
+        <v>0.0361746282580966</v>
       </c>
       <c r="G27" s="0" t="n">
         <f aca="false">G25/B25-1</f>
@@ -17416,11 +17355,11 @@
       </c>
       <c r="H27" s="0" t="n">
         <f aca="false">H25/C25-1</f>
-        <v>0.0097323924320345</v>
+        <v>0.00973239243203472</v>
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">I25/C25-1</f>
-        <v>0.0216797125909778</v>
+        <v>0.0216797125909782</v>
       </c>
       <c r="J27" s="0" t="n">
         <f aca="false">J25/D25-1</f>
@@ -17428,15 +17367,15 @@
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">K25/D25-1</f>
-        <v>0.0322466029673021</v>
+        <v>0.0322466029673023</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">L25/E25-1</f>
-        <v>0.0344631425999624</v>
+        <v>0.0344631425999626</v>
       </c>
       <c r="M27" s="0" t="n">
         <f aca="false">M25/E25-1</f>
-        <v>0.064804872588037</v>
+        <v>0.0648048725880368</v>
       </c>
     </row>
   </sheetData>
@@ -17463,45 +17402,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="15" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="Q1" s="0" t="str">
         <f aca="false">B1</f>
@@ -17553,7 +17494,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5945.402</v>
@@ -17971,7 +17912,7 @@
         <v>21</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">Q3/Q2-1</f>
@@ -18033,7 +17974,7 @@
         <v>5763.675</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>8051.454</v>
@@ -18060,7 +18001,7 @@
         <v>9051.354</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">Q5/Q4-1</f>
@@ -18227,40 +18168,40 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="I12" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="J12" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="K12" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="L12" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18645,40 +18586,40 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="J23" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="K23" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="L23" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18686,7 +18627,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>15479.375</v>
@@ -18920,7 +18861,7 @@
         <v>15147.266</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>19643.771</v>
@@ -19074,40 +19015,40 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="E34" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="G34" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="H34" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="I34" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="J34" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="L34" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19514,13 +19455,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>